<commit_message>
included proper spreadsheet metadata / added CMM tracking template
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/working_material/AVCDL CMMC.xlsx
+++ b/distribution/reference_documents/working_material/AVCDL CMMC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/reference_documents/working_material/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charleswilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2B864A-674B-2143-BD9B-5136CE46CA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8548CA16-BCCB-384A-8750-819CBA60C8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10120" yWindow="3260" windowWidth="54640" windowHeight="24840" xr2:uid="{3436264A-B807-9846-8242-81807EE259D9}"/>
   </bookViews>
@@ -736,6 +736,15 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -757,20 +766,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1110,95 +1110,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="181" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>118</v>
       </c>
       <c r="C1" s="31"/>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="39" t="s">
+      <c r="G1" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="J1" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="K1" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="L1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="M1" s="39" t="s">
+      <c r="M1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="39" t="s">
+      <c r="N1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="O1" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="P1" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="Q1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="S1" s="39" t="s">
+      <c r="S1" s="32" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="U1" s="42" t="s">
+      <c r="U1" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
+      <c r="V1" s="34"/>
+      <c r="W1" s="34"/>
+      <c r="X1" s="34"/>
+      <c r="Y1" s="34"/>
     </row>
     <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
+      <c r="A2" s="43"/>
+      <c r="B2" s="43"/>
       <c r="C2" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
       <c r="U2" s="29">
         <v>1</v>
       </c>
@@ -1216,7 +1216,7 @@
       </c>
     </row>
     <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="41" t="s">
         <v>100</v>
       </c>
       <c r="B3" s="22">
@@ -1253,7 +1253,7 @@
       <c r="Y3" s="10"/>
     </row>
     <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="38"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="22">
         <v>2</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="Y4" s="10"/>
     </row>
     <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -1333,7 +1333,7 @@
       </c>
     </row>
     <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="22">
         <v>4</v>
       </c>
@@ -1368,7 +1368,7 @@
       <c r="Y6" s="10"/>
     </row>
     <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="14">
         <v>5</v>
       </c>
@@ -1415,7 +1415,7 @@
       <c r="Y7" s="10"/>
     </row>
     <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="14">
         <v>6</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="Y8" s="10"/>
     </row>
     <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="22">
         <v>7</v>
       </c>
@@ -1501,7 +1501,7 @@
       </c>
     </row>
     <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="38"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="22">
         <v>8</v>
       </c>
@@ -1538,7 +1538,7 @@
       <c r="Y10" s="10"/>
     </row>
     <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="22">
         <v>9</v>
       </c>
@@ -1577,7 +1577,7 @@
       <c r="Y11" s="10"/>
     </row>
     <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="14">
         <v>10</v>
       </c>
@@ -1641,7 +1641,7 @@
       <c r="Y13" s="16"/>
     </row>
     <row r="14" spans="1:25" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>75</v>
       </c>
       <c r="B14" s="22">
@@ -1680,7 +1680,7 @@
       <c r="Y14" s="10"/>
     </row>
     <row r="15" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="22">
         <v>2</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="Y16" s="16"/>
     </row>
     <row r="17" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="41" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="26">
@@ -1785,7 +1785,7 @@
       </c>
     </row>
     <row r="18" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="22">
         <v>2</v>
       </c>
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="19" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="38"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="22">
         <v>3</v>
       </c>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="20" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="22">
         <v>4</v>
       </c>
@@ -1904,7 +1904,7 @@
       </c>
     </row>
     <row r="21" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="22">
         <v>5</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="Y22" s="16"/>
     </row>
     <row r="23" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="32" t="s">
+      <c r="A23" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="26">
@@ -2007,7 +2007,7 @@
       </c>
     </row>
     <row r="24" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="33"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="14">
         <v>2</v>
       </c>
@@ -2048,7 +2048,7 @@
       </c>
     </row>
     <row r="25" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="33"/>
+      <c r="A25" s="36"/>
       <c r="B25" s="22">
         <v>3</v>
       </c>
@@ -2089,7 +2089,7 @@
       </c>
     </row>
     <row r="26" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="33"/>
+      <c r="A26" s="36"/>
       <c r="B26" s="26">
         <v>4</v>
       </c>
@@ -2120,7 +2120,7 @@
       <c r="Y26" s="10"/>
     </row>
     <row r="27" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="33"/>
+      <c r="A27" s="36"/>
       <c r="B27" s="26">
         <v>5</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="Y27" s="10"/>
     </row>
     <row r="28" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="33"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="26">
         <v>6</v>
       </c>
@@ -2192,7 +2192,7 @@
       <c r="Y28" s="10"/>
     </row>
     <row r="29" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="33"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="14">
         <v>7</v>
       </c>
@@ -2223,7 +2223,7 @@
       <c r="Y29" s="10"/>
     </row>
     <row r="30" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="33"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="26">
         <v>8</v>
       </c>
@@ -2258,7 +2258,7 @@
       </c>
     </row>
     <row r="31" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
+      <c r="A31" s="36"/>
       <c r="B31" s="22">
         <v>9</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
     </row>
     <row r="32" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="33"/>
+      <c r="A32" s="36"/>
       <c r="B32" s="25">
         <v>10</v>
       </c>
@@ -2326,7 +2326,7 @@
       <c r="Y32" s="10"/>
     </row>
     <row r="33" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="34"/>
+      <c r="A33" s="37"/>
       <c r="B33" s="22">
         <v>11</v>
       </c>
@@ -2390,7 +2390,7 @@
       <c r="Y34" s="16"/>
     </row>
     <row r="35" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="38" t="s">
         <v>40</v>
       </c>
       <c r="B35" s="22">
@@ -2427,7 +2427,7 @@
       <c r="Y35" s="10"/>
     </row>
     <row r="36" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="36"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="22">
         <v>2</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="Y36" s="10"/>
     </row>
     <row r="37" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="36"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="22">
         <v>3</v>
       </c>
@@ -2501,7 +2501,7 @@
       <c r="Y37" s="10"/>
     </row>
     <row r="38" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="37"/>
+      <c r="A38" s="40"/>
       <c r="B38" s="22">
         <v>4</v>
       </c>
@@ -2565,7 +2565,7 @@
       <c r="Y39" s="16"/>
     </row>
     <row r="40" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B40" s="22">
@@ -2610,7 +2610,7 @@
       </c>
     </row>
     <row r="41" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="38"/>
+      <c r="A41" s="41"/>
       <c r="B41" s="14">
         <v>2</v>
       </c>
@@ -2653,7 +2653,7 @@
       </c>
     </row>
     <row r="42" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
+      <c r="A42" s="41"/>
       <c r="B42" s="22">
         <v>3</v>
       </c>
@@ -2717,7 +2717,7 @@
       <c r="Y43" s="16"/>
     </row>
     <row r="44" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="41" t="s">
         <v>25</v>
       </c>
       <c r="B44" s="22">
@@ -2766,7 +2766,7 @@
       </c>
     </row>
     <row r="45" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="38"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="22">
         <v>2</v>
       </c>
@@ -2807,7 +2807,7 @@
       <c r="Y45" s="10"/>
     </row>
     <row r="46" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="38"/>
+      <c r="A46" s="41"/>
       <c r="B46" s="22">
         <v>3</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="Y46" s="10"/>
     </row>
     <row r="47" spans="1:25" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="38"/>
+      <c r="A47" s="41"/>
       <c r="B47" s="14">
         <v>4</v>
       </c>
@@ -3014,23 +3014,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
     <mergeCell ref="A23:A33"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A40:A42"/>
@@ -3041,6 +3024,23 @@
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="A17:A21"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:N2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="O1:O2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>